<commit_message>
Added TCs [252734, 252733, 252690]
</commit_message>
<xml_diff>
--- a/West.EnterpriseUX.Automation/West.EnterpriseUX.Automation.MobileNew/TestData/DEV/KPIs_252691.xlsx
+++ b/West.EnterpriseUX.Automation/West.EnterpriseUX.Automation.MobileNew/TestData/DEV/KPIs_252691.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patilg\source\repos\UAT_Test\EnterpriseUX.MobileAutomation\West.EnterpriseUX.Automation\West.EnterpriseUX.Automation.MobileNew\TestData\DEV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6565F3EB-9E40-4335-B83C-05CC9B94EA29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{225058A7-AF1A-48B0-9B88-331466D4E0FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1820" yWindow="1820" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs_252691" sheetId="1" r:id="rId1"/>

</xml_diff>